<commit_message>
added peak map xlsx
</commit_message>
<xml_diff>
--- a/data/isotopes_metadata.xlsx
+++ b/data/isotopes_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tristan/csci/tristan_d2o/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E17857-0C89-684D-B510-9AC7B35C2E30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4080370F-1E45-C243-8273-50D776DD59E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{773A3C63-07D1-B24A-B383-28214255C080}"/>
   </bookViews>
@@ -436,7 +436,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
commit as of 12/28/2019
</commit_message>
<xml_diff>
--- a/data/isotopes_metadata.xlsx
+++ b/data/isotopes_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tristan/csci/tristan_d2o/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4080370F-1E45-C243-8273-50D776DD59E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619C14CE-5240-0745-B3AE-F0697E25D512}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{773A3C63-07D1-B24A-B383-28214255C080}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{773A3C63-07D1-B24A-B383-28214255C080}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>MBX_FAMES</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>id1</t>
+  </si>
+  <si>
+    <t>MAX_FAMES</t>
+  </si>
+  <si>
+    <t>MAW_FAMES</t>
   </si>
 </sst>
 </file>
@@ -116,9 +122,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F4FCC4D-0FD2-084E-AE49-7112B4E0021F}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -462,25 +469,25 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="b">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -489,7 +496,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -497,7 +504,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -506,7 +513,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -514,13 +521,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
       <c r="C5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>50</v>
@@ -531,24 +538,24 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="E6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
@@ -557,7 +564,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -565,7 +572,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
@@ -574,7 +581,7 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
@@ -582,18 +589,52 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>50</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9">
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11">
         <v>50</v>
       </c>
-      <c r="E9" t="b">
+      <c r="E11" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>